<commit_message>
fixed duplicate detection flow to properly find duplicates and create a UI for selecting which value to use'
</commit_message>
<xml_diff>
--- a/tests/data/ece_scholarship_applicants.xlsx
+++ b/tests/data/ece_scholarship_applicants.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mkgarvin/Desktop/ECEScholarshipCommitteeSoftwareTeam/toTeam/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pp-brandon/Projects/team_02/tests/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{4E7A8D26-2A03-8842-BA6D-C0B93A080B41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C260441F-EF6D-4434-AC93-CA7ED6D0F9D4}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0795348-9BE1-F142-B558-26AB2C7D9CAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="29040" windowHeight="15840" xr2:uid="{7F514D49-806D-4E7F-B620-4DF7541FD9DC}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15840" xr2:uid="{7F514D49-806D-4E7F-B620-4DF7541FD9DC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1553" uniqueCount="542">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1554" uniqueCount="543">
   <si>
     <t>Category</t>
   </si>
@@ -1662,13 +1662,16 @@
   </si>
   <si>
     <t>Quisque id justo sit amet sapien dignissim vestibulum. Vestibulum ante ipsum primis in faucibus orci luctus et ultrices posuere cubilia Curae; Nulla dapibus dolor vel est. Donec odio justo, sollicitudin ut, suscipit a, feugiat et, eros. Vestibulum ac est lacinia nisi venenatis tristique. Fusce congue, diam id ornare imperdiet, sapien urna pretium nisl, ut volutpat sapien arcu sed augue. Aliquam erat volutpat.</t>
+  </si>
+  <si>
+    <t>Duplicate</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2013,19 +2016,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{607727F6-1065-4008-BF52-4F6921300BD7}">
-  <dimension ref="A1:W140"/>
+  <dimension ref="A1:X140"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="W1" sqref="W1"/>
+    <sheetView tabSelected="1" topLeftCell="E5" workbookViewId="0">
+      <selection activeCell="W24" sqref="W24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.140625" customWidth="1"/>
-    <col min="2" max="2" width="12.85546875" customWidth="1"/>
+    <col min="1" max="1" width="9.1640625" customWidth="1"/>
+    <col min="2" max="2" width="12.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2093,10 +2096,13 @@
         <v>21</v>
       </c>
       <c r="W1" t="s">
+        <v>542</v>
+      </c>
+      <c r="X1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:23">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>23</v>
       </c>
@@ -2154,11 +2160,14 @@
       <c r="V2" t="s">
         <v>34</v>
       </c>
-      <c r="W2" t="s">
+      <c r="W2">
+        <v>1</v>
+      </c>
+      <c r="X2" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:23">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>23</v>
       </c>
@@ -2216,11 +2225,14 @@
       <c r="V3" t="s">
         <v>34</v>
       </c>
-      <c r="W3" t="s">
+      <c r="W3">
+        <v>1</v>
+      </c>
+      <c r="X3" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="4" spans="1:23">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>23</v>
       </c>
@@ -2275,11 +2287,14 @@
       <c r="V4" t="s">
         <v>34</v>
       </c>
-      <c r="W4" t="s">
+      <c r="W4">
+        <v>1</v>
+      </c>
+      <c r="X4" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="5" spans="1:23">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>23</v>
       </c>
@@ -2334,11 +2349,14 @@
       <c r="V5" t="s">
         <v>34</v>
       </c>
-      <c r="W5" t="s">
+      <c r="W5">
+        <v>3</v>
+      </c>
+      <c r="X5" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="6" spans="1:23">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>23</v>
       </c>
@@ -2393,11 +2411,14 @@
       <c r="V6" t="s">
         <v>34</v>
       </c>
-      <c r="W6" t="s">
+      <c r="W6">
+        <v>1</v>
+      </c>
+      <c r="X6" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="7" spans="1:23">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>23</v>
       </c>
@@ -2452,11 +2473,14 @@
       <c r="V7" t="s">
         <v>34</v>
       </c>
-      <c r="W7" t="s">
+      <c r="W7">
+        <v>1</v>
+      </c>
+      <c r="X7" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="8" spans="1:23">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>23</v>
       </c>
@@ -2511,11 +2535,14 @@
       <c r="V8" t="s">
         <v>34</v>
       </c>
-      <c r="W8" t="s">
+      <c r="W8">
+        <v>1</v>
+      </c>
+      <c r="X8" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="9" spans="1:23">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>23</v>
       </c>
@@ -2570,11 +2597,14 @@
       <c r="V9" t="s">
         <v>34</v>
       </c>
-      <c r="W9" t="s">
+      <c r="W9">
+        <v>1</v>
+      </c>
+      <c r="X9" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="10" spans="1:23">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>23</v>
       </c>
@@ -2629,11 +2659,14 @@
       <c r="V10" t="s">
         <v>34</v>
       </c>
-      <c r="W10" t="s">
+      <c r="W10">
+        <v>1</v>
+      </c>
+      <c r="X10" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="11" spans="1:23">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>23</v>
       </c>
@@ -2691,11 +2724,14 @@
       <c r="V11" t="s">
         <v>34</v>
       </c>
-      <c r="W11" t="s">
+      <c r="W11">
+        <v>1</v>
+      </c>
+      <c r="X11" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="12" spans="1:23">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>23</v>
       </c>
@@ -2753,11 +2789,14 @@
       <c r="V12" t="s">
         <v>34</v>
       </c>
-      <c r="W12" t="s">
+      <c r="W12">
+        <v>1</v>
+      </c>
+      <c r="X12" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="13" spans="1:23">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>23</v>
       </c>
@@ -2812,11 +2851,14 @@
       <c r="V13" t="s">
         <v>34</v>
       </c>
-      <c r="W13" t="s">
+      <c r="W13">
+        <v>1</v>
+      </c>
+      <c r="X13" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="14" spans="1:23">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>23</v>
       </c>
@@ -2874,11 +2916,14 @@
       <c r="V14" t="s">
         <v>34</v>
       </c>
-      <c r="W14" t="s">
+      <c r="W14">
+        <v>1</v>
+      </c>
+      <c r="X14" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="15" spans="1:23">
+    <row r="15" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>23</v>
       </c>
@@ -2936,11 +2981,14 @@
       <c r="V15" t="s">
         <v>34</v>
       </c>
-      <c r="W15" t="s">
+      <c r="W15">
+        <v>1</v>
+      </c>
+      <c r="X15" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="16" spans="1:23">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>23</v>
       </c>
@@ -2998,11 +3046,14 @@
       <c r="V16" t="s">
         <v>34</v>
       </c>
-      <c r="W16" t="s">
+      <c r="W16">
+        <v>1</v>
+      </c>
+      <c r="X16" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="17" spans="1:23">
+    <row r="17" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>23</v>
       </c>
@@ -3060,11 +3111,14 @@
       <c r="V17" t="s">
         <v>34</v>
       </c>
-      <c r="W17" t="s">
+      <c r="W17">
+        <v>1</v>
+      </c>
+      <c r="X17" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="18" spans="1:23">
+    <row r="18" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>23</v>
       </c>
@@ -3125,11 +3179,14 @@
       <c r="V18" t="s">
         <v>34</v>
       </c>
-      <c r="W18" t="s">
+      <c r="W18">
+        <v>1</v>
+      </c>
+      <c r="X18" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="19" spans="1:23">
+    <row r="19" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>23</v>
       </c>
@@ -3184,11 +3241,14 @@
       <c r="V19" t="s">
         <v>34</v>
       </c>
-      <c r="W19" t="s">
+      <c r="W19">
+        <v>1</v>
+      </c>
+      <c r="X19" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="20" spans="1:23">
+    <row r="20" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>23</v>
       </c>
@@ -3246,11 +3306,14 @@
       <c r="V20" t="s">
         <v>34</v>
       </c>
-      <c r="W20" t="s">
+      <c r="W20">
+        <v>1</v>
+      </c>
+      <c r="X20" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="21" spans="1:23">
+    <row r="21" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>23</v>
       </c>
@@ -3308,11 +3371,14 @@
       <c r="V21" t="s">
         <v>34</v>
       </c>
-      <c r="W21" t="s">
+      <c r="W21">
+        <v>1</v>
+      </c>
+      <c r="X21" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="22" spans="1:23">
+    <row r="22" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>23</v>
       </c>
@@ -3370,11 +3436,14 @@
       <c r="V22" t="s">
         <v>34</v>
       </c>
-      <c r="W22" t="s">
+      <c r="W22">
+        <v>1</v>
+      </c>
+      <c r="X22" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="23" spans="1:23">
+    <row r="23" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>23</v>
       </c>
@@ -3429,11 +3498,14 @@
       <c r="V23" t="s">
         <v>34</v>
       </c>
-      <c r="W23" t="s">
+      <c r="W23">
+        <v>1</v>
+      </c>
+      <c r="X23" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="24" spans="1:23">
+    <row r="24" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>23</v>
       </c>
@@ -3491,11 +3563,14 @@
       <c r="V24" t="s">
         <v>34</v>
       </c>
-      <c r="W24" t="s">
+      <c r="W24">
+        <v>2</v>
+      </c>
+      <c r="X24" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="25" spans="1:23">
+    <row r="25" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>23</v>
       </c>
@@ -3553,11 +3628,14 @@
       <c r="V25" t="s">
         <v>34</v>
       </c>
-      <c r="W25" t="s">
+      <c r="W25">
+        <v>1</v>
+      </c>
+      <c r="X25" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="26" spans="1:23">
+    <row r="26" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>23</v>
       </c>
@@ -3618,11 +3696,14 @@
       <c r="V26" t="s">
         <v>34</v>
       </c>
-      <c r="W26" t="s">
+      <c r="W26">
+        <v>1</v>
+      </c>
+      <c r="X26" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="27" spans="1:23">
+    <row r="27" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>23</v>
       </c>
@@ -3680,11 +3761,14 @@
       <c r="V27" t="s">
         <v>34</v>
       </c>
-      <c r="W27" t="s">
+      <c r="W27">
+        <v>1</v>
+      </c>
+      <c r="X27" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="28" spans="1:23">
+    <row r="28" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>23</v>
       </c>
@@ -3742,11 +3826,14 @@
       <c r="V28" t="s">
         <v>34</v>
       </c>
-      <c r="W28" t="s">
+      <c r="W28">
+        <v>1</v>
+      </c>
+      <c r="X28" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="29" spans="1:23">
+    <row r="29" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>23</v>
       </c>
@@ -3804,11 +3891,14 @@
       <c r="V29" t="s">
         <v>34</v>
       </c>
-      <c r="W29" t="s">
+      <c r="W29">
+        <v>1</v>
+      </c>
+      <c r="X29" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="30" spans="1:23">
+    <row r="30" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>23</v>
       </c>
@@ -3866,11 +3956,14 @@
       <c r="V30" t="s">
         <v>34</v>
       </c>
-      <c r="W30" t="s">
+      <c r="W30">
+        <v>1</v>
+      </c>
+      <c r="X30" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="31" spans="1:23">
+    <row r="31" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>23</v>
       </c>
@@ -3925,11 +4018,14 @@
       <c r="V31" t="s">
         <v>34</v>
       </c>
-      <c r="W31" t="s">
+      <c r="W31">
+        <v>1</v>
+      </c>
+      <c r="X31" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="32" spans="1:23">
+    <row r="32" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>23</v>
       </c>
@@ -3987,11 +4083,14 @@
       <c r="V32" t="s">
         <v>34</v>
       </c>
-      <c r="W32" t="s">
+      <c r="W32">
+        <v>1</v>
+      </c>
+      <c r="X32" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="33" spans="1:23">
+    <row r="33" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>23</v>
       </c>
@@ -4055,11 +4154,14 @@
       <c r="V33" t="s">
         <v>34</v>
       </c>
-      <c r="W33" t="s">
+      <c r="W33">
+        <v>1</v>
+      </c>
+      <c r="X33" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="34" spans="1:23">
+    <row r="34" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>23</v>
       </c>
@@ -4123,11 +4225,14 @@
       <c r="V34" t="s">
         <v>34</v>
       </c>
-      <c r="W34" t="s">
+      <c r="W34">
+        <v>1</v>
+      </c>
+      <c r="X34" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="35" spans="1:23">
+    <row r="35" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>23</v>
       </c>
@@ -4185,11 +4290,14 @@
       <c r="V35" t="s">
         <v>34</v>
       </c>
-      <c r="W35" t="s">
+      <c r="W35">
+        <v>1</v>
+      </c>
+      <c r="X35" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="36" spans="1:23">
+    <row r="36" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>23</v>
       </c>
@@ -4247,11 +4355,14 @@
       <c r="V36" t="s">
         <v>34</v>
       </c>
-      <c r="W36" t="s">
+      <c r="W36">
+        <v>1</v>
+      </c>
+      <c r="X36" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="37" spans="1:23">
+    <row r="37" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>23</v>
       </c>
@@ -4309,11 +4420,14 @@
       <c r="V37" t="s">
         <v>34</v>
       </c>
-      <c r="W37" t="s">
+      <c r="W37">
+        <v>1</v>
+      </c>
+      <c r="X37" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="38" spans="1:23">
+    <row r="38" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>23</v>
       </c>
@@ -4368,11 +4482,14 @@
       <c r="V38" t="s">
         <v>34</v>
       </c>
-      <c r="W38" t="s">
+      <c r="W38">
+        <v>1</v>
+      </c>
+      <c r="X38" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="39" spans="1:23">
+    <row r="39" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>23</v>
       </c>
@@ -4427,11 +4544,14 @@
       <c r="V39" t="s">
         <v>34</v>
       </c>
-      <c r="W39" t="s">
+      <c r="W39">
+        <v>1</v>
+      </c>
+      <c r="X39" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="40" spans="1:23">
+    <row r="40" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>23</v>
       </c>
@@ -4489,11 +4609,14 @@
       <c r="V40" t="s">
         <v>34</v>
       </c>
-      <c r="W40" t="s">
+      <c r="W40">
+        <v>1</v>
+      </c>
+      <c r="X40" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="41" spans="1:23">
+    <row r="41" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>23</v>
       </c>
@@ -4548,11 +4671,14 @@
       <c r="V41" t="s">
         <v>34</v>
       </c>
-      <c r="W41" t="s">
+      <c r="W41">
+        <v>1</v>
+      </c>
+      <c r="X41" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="42" spans="1:23">
+    <row r="42" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>23</v>
       </c>
@@ -4610,11 +4736,14 @@
       <c r="V42" t="s">
         <v>34</v>
       </c>
-      <c r="W42" t="s">
+      <c r="W42">
+        <v>1</v>
+      </c>
+      <c r="X42" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="43" spans="1:23">
+    <row r="43" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>23</v>
       </c>
@@ -4672,11 +4801,14 @@
       <c r="V43" t="s">
         <v>34</v>
       </c>
-      <c r="W43" t="s">
+      <c r="W43">
+        <v>1</v>
+      </c>
+      <c r="X43" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="44" spans="1:23">
+    <row r="44" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>23</v>
       </c>
@@ -4731,11 +4863,14 @@
       <c r="V44" t="s">
         <v>34</v>
       </c>
-      <c r="W44" t="s">
+      <c r="W44">
+        <v>1</v>
+      </c>
+      <c r="X44" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="45" spans="1:23">
+    <row r="45" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>23</v>
       </c>
@@ -4790,11 +4925,14 @@
       <c r="V45" t="s">
         <v>34</v>
       </c>
-      <c r="W45" t="s">
+      <c r="W45">
+        <v>1</v>
+      </c>
+      <c r="X45" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="46" spans="1:23">
+    <row r="46" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>23</v>
       </c>
@@ -4852,11 +4990,14 @@
       <c r="V46" t="s">
         <v>34</v>
       </c>
-      <c r="W46" t="s">
+      <c r="W46">
+        <v>1</v>
+      </c>
+      <c r="X46" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="47" spans="1:23">
+    <row r="47" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>23</v>
       </c>
@@ -4911,11 +5052,14 @@
       <c r="V47" t="s">
         <v>34</v>
       </c>
-      <c r="W47" t="s">
+      <c r="W47">
+        <v>1</v>
+      </c>
+      <c r="X47" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="48" spans="1:23">
+    <row r="48" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>23</v>
       </c>
@@ -4970,11 +5114,14 @@
       <c r="V48" t="s">
         <v>34</v>
       </c>
-      <c r="W48" t="s">
+      <c r="W48">
+        <v>1</v>
+      </c>
+      <c r="X48" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="49" spans="1:23">
+    <row r="49" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>23</v>
       </c>
@@ -5029,11 +5176,14 @@
       <c r="V49" t="s">
         <v>34</v>
       </c>
-      <c r="W49" t="s">
+      <c r="W49">
+        <v>1</v>
+      </c>
+      <c r="X49" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="50" spans="1:23">
+    <row r="50" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>23</v>
       </c>
@@ -5091,11 +5241,14 @@
       <c r="V50" t="s">
         <v>34</v>
       </c>
-      <c r="W50" t="s">
+      <c r="W50">
+        <v>1</v>
+      </c>
+      <c r="X50" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="51" spans="1:23">
+    <row r="51" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>23</v>
       </c>
@@ -5153,11 +5306,14 @@
       <c r="V51" t="s">
         <v>34</v>
       </c>
-      <c r="W51" t="s">
+      <c r="W51">
+        <v>1</v>
+      </c>
+      <c r="X51" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="52" spans="1:23">
+    <row r="52" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>23</v>
       </c>
@@ -5215,11 +5371,14 @@
       <c r="V52" t="s">
         <v>34</v>
       </c>
-      <c r="W52" t="s">
+      <c r="W52">
+        <v>1</v>
+      </c>
+      <c r="X52" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="53" spans="1:23">
+    <row r="53" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>23</v>
       </c>
@@ -5277,11 +5436,14 @@
       <c r="V53" t="s">
         <v>34</v>
       </c>
-      <c r="W53" t="s">
+      <c r="W53">
+        <v>1</v>
+      </c>
+      <c r="X53" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="54" spans="1:23">
+    <row r="54" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>23</v>
       </c>
@@ -5339,11 +5501,14 @@
       <c r="V54" t="s">
         <v>34</v>
       </c>
-      <c r="W54" t="s">
+      <c r="W54">
+        <v>1</v>
+      </c>
+      <c r="X54" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="55" spans="1:23">
+    <row r="55" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>23</v>
       </c>
@@ -5401,11 +5566,14 @@
       <c r="V55" t="s">
         <v>34</v>
       </c>
-      <c r="W55" t="s">
+      <c r="W55">
+        <v>1</v>
+      </c>
+      <c r="X55" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="56" spans="1:23">
+    <row r="56" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>274</v>
       </c>
@@ -5463,11 +5631,14 @@
       <c r="V56" t="s">
         <v>34</v>
       </c>
-      <c r="W56" t="s">
+      <c r="W56">
+        <v>1</v>
+      </c>
+      <c r="X56" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="57" spans="1:23">
+    <row r="57" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>274</v>
       </c>
@@ -5525,11 +5696,14 @@
       <c r="V57" t="s">
         <v>34</v>
       </c>
-      <c r="W57" t="s">
+      <c r="W57">
+        <v>1</v>
+      </c>
+      <c r="X57" t="s">
         <v>283</v>
       </c>
     </row>
-    <row r="58" spans="1:23">
+    <row r="58" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>274</v>
       </c>
@@ -5587,11 +5761,14 @@
       <c r="V58" t="s">
         <v>34</v>
       </c>
-      <c r="W58" t="s">
+      <c r="W58">
+        <v>1</v>
+      </c>
+      <c r="X58" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="59" spans="1:23">
+    <row r="59" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>274</v>
       </c>
@@ -5649,11 +5826,14 @@
       <c r="V59" t="s">
         <v>34</v>
       </c>
-      <c r="W59" t="s">
+      <c r="W59">
+        <v>1</v>
+      </c>
+      <c r="X59" t="s">
         <v>289</v>
       </c>
     </row>
-    <row r="60" spans="1:23">
+    <row r="60" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>274</v>
       </c>
@@ -5708,11 +5888,14 @@
       <c r="V60" t="s">
         <v>34</v>
       </c>
-      <c r="W60" t="s">
+      <c r="W60">
+        <v>1</v>
+      </c>
+      <c r="X60" t="s">
         <v>294</v>
       </c>
     </row>
-    <row r="61" spans="1:23">
+    <row r="61" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>274</v>
       </c>
@@ -5767,11 +5950,14 @@
       <c r="V61" t="s">
         <v>34</v>
       </c>
-      <c r="W61" t="s">
+      <c r="W61">
+        <v>1</v>
+      </c>
+      <c r="X61" t="s">
         <v>298</v>
       </c>
     </row>
-    <row r="62" spans="1:23">
+    <row r="62" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>274</v>
       </c>
@@ -5829,11 +6015,14 @@
       <c r="V62" t="s">
         <v>34</v>
       </c>
-      <c r="W62" t="s">
+      <c r="W62">
+        <v>1</v>
+      </c>
+      <c r="X62" t="s">
         <v>301</v>
       </c>
     </row>
-    <row r="63" spans="1:23">
+    <row r="63" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>274</v>
       </c>
@@ -5888,11 +6077,14 @@
       <c r="V63" t="s">
         <v>34</v>
       </c>
-      <c r="W63" t="s">
+      <c r="W63">
+        <v>1</v>
+      </c>
+      <c r="X63" t="s">
         <v>306</v>
       </c>
     </row>
-    <row r="64" spans="1:23">
+    <row r="64" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>274</v>
       </c>
@@ -5950,11 +6142,14 @@
       <c r="V64" t="s">
         <v>34</v>
       </c>
-      <c r="W64" t="s">
+      <c r="W64">
+        <v>1</v>
+      </c>
+      <c r="X64" t="s">
         <v>309</v>
       </c>
     </row>
-    <row r="65" spans="1:23">
+    <row r="65" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>274</v>
       </c>
@@ -6012,11 +6207,14 @@
       <c r="V65" t="s">
         <v>34</v>
       </c>
-      <c r="W65" t="s">
+      <c r="W65">
+        <v>1</v>
+      </c>
+      <c r="X65" t="s">
         <v>313</v>
       </c>
     </row>
-    <row r="66" spans="1:23">
+    <row r="66" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>274</v>
       </c>
@@ -6074,11 +6272,14 @@
       <c r="V66" t="s">
         <v>34</v>
       </c>
-      <c r="W66" t="s">
+      <c r="W66">
+        <v>1</v>
+      </c>
+      <c r="X66" t="s">
         <v>316</v>
       </c>
     </row>
-    <row r="67" spans="1:23">
+    <row r="67" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>274</v>
       </c>
@@ -6136,11 +6337,14 @@
       <c r="V67" t="s">
         <v>34</v>
       </c>
-      <c r="W67" t="s">
+      <c r="W67">
+        <v>1</v>
+      </c>
+      <c r="X67" t="s">
         <v>320</v>
       </c>
     </row>
-    <row r="68" spans="1:23">
+    <row r="68" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>274</v>
       </c>
@@ -6198,11 +6402,14 @@
       <c r="V68" t="s">
         <v>34</v>
       </c>
-      <c r="W68" t="s">
+      <c r="W68">
+        <v>1</v>
+      </c>
+      <c r="X68" t="s">
         <v>324</v>
       </c>
     </row>
-    <row r="69" spans="1:23">
+    <row r="69" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>274</v>
       </c>
@@ -6257,11 +6464,14 @@
       <c r="V69" t="s">
         <v>34</v>
       </c>
-      <c r="W69" t="s">
+      <c r="W69">
+        <v>1</v>
+      </c>
+      <c r="X69" t="s">
         <v>327</v>
       </c>
     </row>
-    <row r="70" spans="1:23">
+    <row r="70" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>274</v>
       </c>
@@ -6319,11 +6529,14 @@
       <c r="V70" t="s">
         <v>34</v>
       </c>
-      <c r="W70" t="s">
+      <c r="W70">
+        <v>1</v>
+      </c>
+      <c r="X70" t="s">
         <v>331</v>
       </c>
     </row>
-    <row r="71" spans="1:23">
+    <row r="71" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>274</v>
       </c>
@@ -6381,11 +6594,14 @@
       <c r="V71" t="s">
         <v>34</v>
       </c>
-      <c r="W71" t="s">
+      <c r="W71">
+        <v>1</v>
+      </c>
+      <c r="X71" t="s">
         <v>336</v>
       </c>
     </row>
-    <row r="72" spans="1:23">
+    <row r="72" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>274</v>
       </c>
@@ -6446,11 +6662,14 @@
       <c r="V72" t="s">
         <v>34</v>
       </c>
-      <c r="W72" t="s">
+      <c r="W72">
+        <v>1</v>
+      </c>
+      <c r="X72" t="s">
         <v>341</v>
       </c>
     </row>
-    <row r="73" spans="1:23">
+    <row r="73" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>274</v>
       </c>
@@ -6511,11 +6730,14 @@
       <c r="V73" t="s">
         <v>34</v>
       </c>
-      <c r="W73" t="s">
+      <c r="W73">
+        <v>1</v>
+      </c>
+      <c r="X73" t="s">
         <v>347</v>
       </c>
     </row>
-    <row r="74" spans="1:23">
+    <row r="74" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>274</v>
       </c>
@@ -6579,11 +6801,14 @@
       <c r="V74" t="s">
         <v>34</v>
       </c>
-      <c r="W74" t="s">
+      <c r="W74">
+        <v>1</v>
+      </c>
+      <c r="X74" t="s">
         <v>352</v>
       </c>
     </row>
-    <row r="75" spans="1:23">
+    <row r="75" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>274</v>
       </c>
@@ -6647,11 +6872,14 @@
       <c r="V75" t="s">
         <v>34</v>
       </c>
-      <c r="W75" t="s">
+      <c r="W75">
+        <v>1</v>
+      </c>
+      <c r="X75" t="s">
         <v>357</v>
       </c>
     </row>
-    <row r="76" spans="1:23">
+    <row r="76" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>274</v>
       </c>
@@ -6715,11 +6943,14 @@
       <c r="V76" t="s">
         <v>34</v>
       </c>
-      <c r="W76" t="s">
+      <c r="W76">
+        <v>1</v>
+      </c>
+      <c r="X76" t="s">
         <v>362</v>
       </c>
     </row>
-    <row r="77" spans="1:23">
+    <row r="77" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>274</v>
       </c>
@@ -6783,11 +7014,14 @@
       <c r="V77" t="s">
         <v>34</v>
       </c>
-      <c r="W77" t="s">
+      <c r="W77">
+        <v>1</v>
+      </c>
+      <c r="X77" t="s">
         <v>368</v>
       </c>
     </row>
-    <row r="78" spans="1:23">
+    <row r="78" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>274</v>
       </c>
@@ -6848,11 +7082,14 @@
       <c r="V78" t="s">
         <v>34</v>
       </c>
-      <c r="W78" t="s">
+      <c r="W78">
+        <v>1</v>
+      </c>
+      <c r="X78" t="s">
         <v>374</v>
       </c>
     </row>
-    <row r="79" spans="1:23">
+    <row r="79" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>274</v>
       </c>
@@ -6913,11 +7150,14 @@
       <c r="V79" t="s">
         <v>34</v>
       </c>
-      <c r="W79" t="s">
+      <c r="W79">
+        <v>1</v>
+      </c>
+      <c r="X79" t="s">
         <v>378</v>
       </c>
     </row>
-    <row r="80" spans="1:23">
+    <row r="80" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>274</v>
       </c>
@@ -6984,11 +7224,14 @@
       <c r="V80" t="s">
         <v>383</v>
       </c>
-      <c r="W80" t="s">
+      <c r="W80">
+        <v>1</v>
+      </c>
+      <c r="X80" t="s">
         <v>384</v>
       </c>
     </row>
-    <row r="81" spans="1:23">
+    <row r="81" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>274</v>
       </c>
@@ -7052,11 +7295,14 @@
       <c r="V81" t="s">
         <v>34</v>
       </c>
-      <c r="W81" t="s">
+      <c r="W81">
+        <v>1</v>
+      </c>
+      <c r="X81" t="s">
         <v>389</v>
       </c>
     </row>
-    <row r="82" spans="1:23">
+    <row r="82" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>274</v>
       </c>
@@ -7117,11 +7363,14 @@
       <c r="V82" t="s">
         <v>34</v>
       </c>
-      <c r="W82" t="s">
+      <c r="W82">
+        <v>1</v>
+      </c>
+      <c r="X82" t="s">
         <v>395</v>
       </c>
     </row>
-    <row r="83" spans="1:23">
+    <row r="83" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>274</v>
       </c>
@@ -7185,11 +7434,14 @@
       <c r="V83" t="s">
         <v>34</v>
       </c>
-      <c r="W83" t="s">
+      <c r="W83">
+        <v>1</v>
+      </c>
+      <c r="X83" t="s">
         <v>401</v>
       </c>
     </row>
-    <row r="84" spans="1:23">
+    <row r="84" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>274</v>
       </c>
@@ -7256,11 +7508,14 @@
       <c r="V84" t="s">
         <v>34</v>
       </c>
-      <c r="W84" t="s">
+      <c r="W84">
+        <v>1</v>
+      </c>
+      <c r="X84" t="s">
         <v>407</v>
       </c>
     </row>
-    <row r="85" spans="1:23">
+    <row r="85" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>274</v>
       </c>
@@ -7324,11 +7579,14 @@
       <c r="V85" t="s">
         <v>34</v>
       </c>
-      <c r="W85" t="s">
+      <c r="W85">
+        <v>1</v>
+      </c>
+      <c r="X85" t="s">
         <v>412</v>
       </c>
     </row>
-    <row r="86" spans="1:23">
+    <row r="86" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>274</v>
       </c>
@@ -7386,11 +7644,14 @@
       <c r="V86" t="s">
         <v>34</v>
       </c>
-      <c r="W86" t="s">
+      <c r="W86">
+        <v>1</v>
+      </c>
+      <c r="X86" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="87" spans="1:23">
+    <row r="87" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>274</v>
       </c>
@@ -7457,11 +7718,14 @@
       <c r="V87" t="s">
         <v>34</v>
       </c>
-      <c r="W87" t="s">
+      <c r="W87">
+        <v>1</v>
+      </c>
+      <c r="X87" t="s">
         <v>419</v>
       </c>
     </row>
-    <row r="88" spans="1:23">
+    <row r="88" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>274</v>
       </c>
@@ -7519,11 +7783,14 @@
       <c r="V88" t="s">
         <v>34</v>
       </c>
-      <c r="W88" t="s">
+      <c r="W88">
+        <v>1</v>
+      </c>
+      <c r="X88" t="s">
         <v>347</v>
       </c>
     </row>
-    <row r="89" spans="1:23">
+    <row r="89" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>274</v>
       </c>
@@ -7587,11 +7854,14 @@
       <c r="V89" t="s">
         <v>34</v>
       </c>
-      <c r="W89" t="s">
+      <c r="W89">
+        <v>1</v>
+      </c>
+      <c r="X89" t="s">
         <v>428</v>
       </c>
     </row>
-    <row r="90" spans="1:23">
+    <row r="90" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>274</v>
       </c>
@@ -7658,11 +7928,14 @@
       <c r="V90" t="s">
         <v>34</v>
       </c>
-      <c r="W90" t="s">
+      <c r="W90">
+        <v>1</v>
+      </c>
+      <c r="X90" t="s">
         <v>434</v>
       </c>
     </row>
-    <row r="91" spans="1:23">
+    <row r="91" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>274</v>
       </c>
@@ -7729,11 +8002,14 @@
       <c r="V91" t="s">
         <v>34</v>
       </c>
-      <c r="W91" t="s">
+      <c r="W91">
+        <v>1</v>
+      </c>
+      <c r="X91" t="s">
         <v>441</v>
       </c>
     </row>
-    <row r="92" spans="1:23">
+    <row r="92" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>274</v>
       </c>
@@ -7800,11 +8076,14 @@
       <c r="V92" t="s">
         <v>34</v>
       </c>
-      <c r="W92" t="s">
+      <c r="W92">
+        <v>1</v>
+      </c>
+      <c r="X92" t="s">
         <v>447</v>
       </c>
     </row>
-    <row r="93" spans="1:23">
+    <row r="93" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>274</v>
       </c>
@@ -7871,11 +8150,14 @@
       <c r="V93" t="s">
         <v>34</v>
       </c>
-      <c r="W93" t="s">
+      <c r="W93">
+        <v>1</v>
+      </c>
+      <c r="X93" t="s">
         <v>452</v>
       </c>
     </row>
-    <row r="94" spans="1:23">
+    <row r="94" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>274</v>
       </c>
@@ -7942,11 +8224,14 @@
       <c r="V94" t="s">
         <v>34</v>
       </c>
-      <c r="W94" t="s">
+      <c r="W94">
+        <v>1</v>
+      </c>
+      <c r="X94" t="s">
         <v>458</v>
       </c>
     </row>
-    <row r="95" spans="1:23">
+    <row r="95" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>274</v>
       </c>
@@ -8013,11 +8298,14 @@
       <c r="V95" t="s">
         <v>383</v>
       </c>
-      <c r="W95" t="s">
+      <c r="W95">
+        <v>1</v>
+      </c>
+      <c r="X95" t="s">
         <v>464</v>
       </c>
     </row>
-    <row r="96" spans="1:23">
+    <row r="96" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>274</v>
       </c>
@@ -8078,11 +8366,14 @@
       <c r="V96" t="s">
         <v>34</v>
       </c>
-      <c r="W96" t="s">
+      <c r="W96">
+        <v>1</v>
+      </c>
+      <c r="X96" t="s">
         <v>468</v>
       </c>
     </row>
-    <row r="97" spans="1:23">
+    <row r="97" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>274</v>
       </c>
@@ -8146,11 +8437,14 @@
       <c r="V97" t="s">
         <v>34</v>
       </c>
-      <c r="W97" t="s">
+      <c r="W97">
+        <v>1</v>
+      </c>
+      <c r="X97" t="s">
         <v>473</v>
       </c>
     </row>
-    <row r="98" spans="1:23">
+    <row r="98" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>274</v>
       </c>
@@ -8217,11 +8511,14 @@
       <c r="V98" t="s">
         <v>34</v>
       </c>
-      <c r="W98" t="s">
+      <c r="W98">
+        <v>1</v>
+      </c>
+      <c r="X98" t="s">
         <v>478</v>
       </c>
     </row>
-    <row r="99" spans="1:23">
+    <row r="99" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>274</v>
       </c>
@@ -8285,11 +8582,14 @@
       <c r="V99" t="s">
         <v>34</v>
       </c>
-      <c r="W99" t="s">
+      <c r="W99">
+        <v>1</v>
+      </c>
+      <c r="X99" t="s">
         <v>484</v>
       </c>
     </row>
-    <row r="100" spans="1:23">
+    <row r="100" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>274</v>
       </c>
@@ -8353,11 +8653,14 @@
       <c r="V100" t="s">
         <v>34</v>
       </c>
-      <c r="W100" t="s">
+      <c r="W100">
+        <v>1</v>
+      </c>
+      <c r="X100" t="s">
         <v>490</v>
       </c>
     </row>
-    <row r="101" spans="1:23">
+    <row r="101" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>274</v>
       </c>
@@ -8421,11 +8724,14 @@
       <c r="V101" t="s">
         <v>34</v>
       </c>
-      <c r="W101" t="s">
+      <c r="W101">
+        <v>1</v>
+      </c>
+      <c r="X101" t="s">
         <v>493</v>
       </c>
     </row>
-    <row r="102" spans="1:23">
+    <row r="102" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>274</v>
       </c>
@@ -8492,11 +8798,14 @@
       <c r="V102" t="s">
         <v>34</v>
       </c>
-      <c r="W102" t="s">
+      <c r="W102">
+        <v>1</v>
+      </c>
+      <c r="X102" t="s">
         <v>498</v>
       </c>
     </row>
-    <row r="103" spans="1:23">
+    <row r="103" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>274</v>
       </c>
@@ -8560,11 +8869,14 @@
       <c r="V103" t="s">
         <v>34</v>
       </c>
-      <c r="W103" t="s">
+      <c r="W103">
+        <v>1</v>
+      </c>
+      <c r="X103" t="s">
         <v>503</v>
       </c>
     </row>
-    <row r="104" spans="1:23">
+    <row r="104" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>274</v>
       </c>
@@ -8625,11 +8937,14 @@
       <c r="V104" t="s">
         <v>34</v>
       </c>
-      <c r="W104" t="s">
+      <c r="W104">
+        <v>1</v>
+      </c>
+      <c r="X104" t="s">
         <v>508</v>
       </c>
     </row>
-    <row r="105" spans="1:23">
+    <row r="105" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>23</v>
       </c>
@@ -8687,11 +9002,14 @@
       <c r="V105" t="s">
         <v>34</v>
       </c>
-      <c r="W105" t="s">
+      <c r="W105">
+        <v>1</v>
+      </c>
+      <c r="X105" t="s">
         <v>512</v>
       </c>
     </row>
-    <row r="106" spans="1:23">
+    <row r="106" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>23</v>
       </c>
@@ -8746,11 +9064,14 @@
       <c r="V106" t="s">
         <v>34</v>
       </c>
-      <c r="W106" t="s">
+      <c r="W106">
+        <v>1</v>
+      </c>
+      <c r="X106" t="s">
         <v>516</v>
       </c>
     </row>
-    <row r="107" spans="1:23">
+    <row r="107" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>23</v>
       </c>
@@ -8805,11 +9126,14 @@
       <c r="V107" t="s">
         <v>34</v>
       </c>
-      <c r="W107" t="s">
+      <c r="W107">
+        <v>1</v>
+      </c>
+      <c r="X107" t="s">
         <v>520</v>
       </c>
     </row>
-    <row r="108" spans="1:23">
+    <row r="108" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>23</v>
       </c>
@@ -8864,11 +9188,14 @@
       <c r="V108" t="s">
         <v>34</v>
       </c>
-      <c r="W108" t="s">
+      <c r="W108">
+        <v>1</v>
+      </c>
+      <c r="X108" t="s">
         <v>524</v>
       </c>
     </row>
-    <row r="109" spans="1:23">
+    <row r="109" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>23</v>
       </c>
@@ -8926,11 +9253,14 @@
       <c r="V109" t="s">
         <v>34</v>
       </c>
-      <c r="W109" t="s">
+      <c r="W109">
+        <v>1</v>
+      </c>
+      <c r="X109" t="s">
         <v>528</v>
       </c>
     </row>
-    <row r="110" spans="1:23">
+    <row r="110" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>23</v>
       </c>
@@ -8985,11 +9315,14 @@
       <c r="V110" t="s">
         <v>34</v>
       </c>
-      <c r="W110" t="s">
+      <c r="W110">
+        <v>1</v>
+      </c>
+      <c r="X110" t="s">
         <v>531</v>
       </c>
     </row>
-    <row r="111" spans="1:23">
+    <row r="111" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>23</v>
       </c>
@@ -9047,11 +9380,14 @@
       <c r="V111" t="s">
         <v>34</v>
       </c>
-      <c r="W111" t="s">
+      <c r="W111">
+        <v>1</v>
+      </c>
+      <c r="X111" t="s">
         <v>534</v>
       </c>
     </row>
-    <row r="112" spans="1:23">
+    <row r="112" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>274</v>
       </c>
@@ -9115,11 +9451,14 @@
       <c r="V112" t="s">
         <v>34</v>
       </c>
-      <c r="W112" t="s">
+      <c r="W112">
+        <v>1</v>
+      </c>
+      <c r="X112" t="s">
         <v>541</v>
       </c>
     </row>
-    <row r="132" spans="19:20">
+    <row r="132" spans="19:20" x14ac:dyDescent="0.2">
       <c r="S132" t="s">
         <v>293</v>
       </c>
@@ -9127,7 +9466,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="133" spans="19:20">
+    <row r="133" spans="19:20" x14ac:dyDescent="0.2">
       <c r="S133" t="s">
         <v>293</v>
       </c>
@@ -9135,7 +9474,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="134" spans="19:20">
+    <row r="134" spans="19:20" x14ac:dyDescent="0.2">
       <c r="S134" t="s">
         <v>293</v>
       </c>
@@ -9143,7 +9482,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="135" spans="19:20">
+    <row r="135" spans="19:20" x14ac:dyDescent="0.2">
       <c r="S135" t="s">
         <v>293</v>
       </c>
@@ -9151,7 +9490,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="136" spans="19:20">
+    <row r="136" spans="19:20" x14ac:dyDescent="0.2">
       <c r="S136" t="s">
         <v>293</v>
       </c>
@@ -9159,7 +9498,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="137" spans="19:20">
+    <row r="137" spans="19:20" x14ac:dyDescent="0.2">
       <c r="S137" t="s">
         <v>293</v>
       </c>
@@ -9167,7 +9506,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="138" spans="19:20">
+    <row r="138" spans="19:20" x14ac:dyDescent="0.2">
       <c r="S138" t="s">
         <v>293</v>
       </c>
@@ -9175,7 +9514,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="139" spans="19:20">
+    <row r="139" spans="19:20" x14ac:dyDescent="0.2">
       <c r="S139" t="s">
         <v>293</v>
       </c>
@@ -9183,7 +9522,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="140" spans="19:20">
+    <row r="140" spans="19:20" x14ac:dyDescent="0.2">
       <c r="S140" t="s">
         <v>293</v>
       </c>
@@ -9206,16 +9545,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="9c9583b9-c8f1-4812-a407-cb17b9992083">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101000C1493E9151C844E8041E39A2FED7C32" ma:contentTypeVersion="8" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d63cc2e3768f676e183991b6485397ed">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="9c9583b9-c8f1-4812-a407-cb17b9992083" xmlns:ns3="af245a6f-3f79-4067-b7ed-91fc345b72bf" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9fe84bd4c9eaf43ec7edf6af3d8203de" ns2:_="" ns3:_="">
     <xsd:import namespace="9c9583b9-c8f1-4812-a407-cb17b9992083"/>
@@ -9400,14 +9729,49 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="9c9583b9-c8f1-4812-a407-cb17b9992083">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9BF33B28-5607-4E19-97AA-5745C95D41C1}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9BF33B28-5607-4E19-97AA-5745C95D41C1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A85815A1-9063-44C8-9DCE-B11ABBB106DA}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{10554743-C4FD-4A46-87F1-55E2958F932B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="9c9583b9-c8f1-4812-a407-cb17b9992083"/>
+    <ds:schemaRef ds:uri="af245a6f-3f79-4067-b7ed-91fc345b72bf"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{10554743-C4FD-4A46-87F1-55E2958F932B}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A85815A1-9063-44C8-9DCE-B11ABBB106DA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="9c9583b9-c8f1-4812-a407-cb17b9992083"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>